<commit_message>
pie chart animation added
</commit_message>
<xml_diff>
--- a/ChartConfig.xlsx
+++ b/ChartConfig.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/moneyPlanner/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE4F7A1-2692-2D40-B93E-46B01038B29A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C338ED-008C-2141-BA0B-E42B4915B9E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19120" xr2:uid="{28808B85-253A-814A-BAB0-EEA512932E88}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="47">
   <si>
     <t>width</t>
   </si>
@@ -173,6 +173,9 @@
   </si>
   <si>
     <t>lineColor</t>
+  </si>
+  <si>
+    <t>className</t>
   </si>
 </sst>
 </file>
@@ -577,11 +580,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC09B64-DEFB-8B44-8394-B651F018A474}">
-  <dimension ref="A1:AD27"/>
+  <dimension ref="A1:AE27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A8" sqref="A8"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -611,10 +614,10 @@
     <col min="27" max="27" width="10.5" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>42</v>
       </c>
@@ -705,8 +708,11 @@
       <c r="AD1" s="4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:30" ht="18" x14ac:dyDescent="0.2">
+      <c r="AE1" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>27</v>
       </c>
@@ -793,7 +799,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>28</v>
       </c>
@@ -856,7 +862,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:30" ht="19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>29</v>
       </c>
@@ -925,7 +931,7 @@
       </c>
       <c r="AC4" s="6"/>
     </row>
-    <row r="5" spans="1:30" ht="19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>30</v>
       </c>
@@ -984,7 +990,7 @@
       </c>
       <c r="AC5" s="6"/>
     </row>
-    <row r="6" spans="1:30" ht="19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>31</v>
       </c>
@@ -1055,7 +1061,7 @@
       </c>
       <c r="AC6" s="6"/>
     </row>
-    <row r="7" spans="1:30" ht="19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>32</v>
       </c>
@@ -1132,7 +1138,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:30" ht="18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:31" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>43</v>
       </c>
@@ -1178,29 +1184,32 @@
       <c r="AD8" s="6" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AE8" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B9" s="1"/>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B16" s="1"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
style changed as object
</commit_message>
<xml_diff>
--- a/ChartConfig.xlsx
+++ b/ChartConfig.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/moneyPlanner/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C338ED-008C-2141-BA0B-E42B4915B9E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33248907-1E16-214F-A709-5DD313A19A9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19120" xr2:uid="{28808B85-253A-814A-BAB0-EEA512932E88}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="47">
   <si>
     <t>width</t>
   </si>
@@ -225,18 +225,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7AC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -251,15 +245,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -583,8 +574,8 @@
   <dimension ref="A1:AE27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D16" sqref="D16"/>
+      <pane xSplit="1" topLeftCell="S1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Y15" sqref="Y15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -598,7 +589,7 @@
     <col min="9" max="9" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="14.5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9.1640625" bestFit="1" customWidth="1"/>
@@ -618,573 +609,576 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="V1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="W1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="X1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Y1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="Z1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AA1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AB1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AC1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AD1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AE1" s="3" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q2" s="6" t="s">
+      <c r="B2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="R2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="T2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="U2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="V2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="W2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="X2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z2" s="6" t="s">
+      <c r="R2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="W2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AA2" s="6" t="s">
+      <c r="AA2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AB2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="AC2" s="6" t="s">
+      <c r="AB2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC2" s="4" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:31" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="7" t="s">
+      <c r="B3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6" t="s">
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="R3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="S3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="V3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="W3" s="6"/>
-      <c r="X3" s="6"/>
-      <c r="Y3" s="6"/>
-      <c r="Z3" s="8"/>
-      <c r="AA3" s="6"/>
-      <c r="AB3" s="6"/>
-      <c r="AC3" s="6" t="s">
+      <c r="R3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="V3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="W3" s="4"/>
+      <c r="X3" s="4"/>
+      <c r="Y3" s="4"/>
+      <c r="Z3" s="5"/>
+      <c r="AA3" s="4"/>
+      <c r="AB3" s="4"/>
+      <c r="AC3" s="4" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:31" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="P4" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q4" s="6" t="s">
+      <c r="B4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q4" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="R4" s="6"/>
-      <c r="S4" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="T4" s="6"/>
-      <c r="U4" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="V4" s="6"/>
-      <c r="W4" s="6"/>
-      <c r="X4" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y4" s="6"/>
-      <c r="Z4" s="8"/>
-      <c r="AA4" s="6" t="s">
+      <c r="R4" s="4"/>
+      <c r="S4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="V4" s="4"/>
+      <c r="W4" s="4"/>
+      <c r="X4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y4" s="4"/>
+      <c r="Z4" s="5"/>
+      <c r="AA4" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AB4" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="AC4" s="6"/>
+      <c r="AB4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC4" s="4"/>
     </row>
     <row r="5" spans="1:31" ht="19" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6" t="s">
+      <c r="B5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="O5" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="P5" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q5" s="6" t="s">
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="M5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="R5" s="6"/>
-      <c r="S5" s="6"/>
-      <c r="T5" s="6"/>
-      <c r="U5" s="6"/>
-      <c r="V5" s="6"/>
-      <c r="W5" s="6"/>
-      <c r="X5" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y5" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z5" s="8"/>
-      <c r="AA5" s="6" t="s">
+      <c r="N5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+      <c r="V5" s="4"/>
+      <c r="W5" s="4"/>
+      <c r="X5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z5" s="5"/>
+      <c r="AA5" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AB5" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="AC5" s="6"/>
+      <c r="AB5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC5" s="4"/>
     </row>
     <row r="6" spans="1:31" ht="19" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="N6" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="O6" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="P6" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q6" s="6" t="s">
+      <c r="B6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q6" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="R6" s="6"/>
-      <c r="S6" s="6"/>
-      <c r="T6" s="6"/>
-      <c r="U6" s="6"/>
-      <c r="V6" s="6"/>
-      <c r="W6" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="X6" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y6" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z6" s="8"/>
-      <c r="AA6" s="6" t="s">
+      <c r="R6" s="4"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
+      <c r="V6" s="4"/>
+      <c r="W6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="X6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z6" s="5"/>
+      <c r="AA6" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AB6" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="AC6" s="6"/>
+      <c r="AB6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC6" s="4"/>
     </row>
     <row r="7" spans="1:31" ht="19" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="M7" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q7" s="6" t="s">
+      <c r="B7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q7" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="R7" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="S7" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="T7" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="U7" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="V7" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="W7" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="X7" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y7" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z7" s="8"/>
-      <c r="AA7" s="6" t="s">
+      <c r="R7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="U7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="V7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="W7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="X7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z7" s="5"/>
+      <c r="AA7" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AB7" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="AC7" s="6" t="s">
+      <c r="AB7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC7" s="4" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:31" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="M8" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="N8" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="O8" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="P8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q8" s="6" t="s">
+      <c r="B8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="P8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q8" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="T8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="V8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="W8" s="6" t="s">
+      <c r="T8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="V8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="W8" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AA8" s="6" t="s">
+      <c r="X8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA8" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AB8" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="AD8" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="AE8" s="6" t="s">
+      <c r="AB8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE8" s="4" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>